<commit_message>
add lmplicit learning module
</commit_message>
<xml_diff>
--- a/vignettes/course_docs/Spring_2022_schedule.xlsx
+++ b/vignettes/course_docs/Spring_2022_schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattcrump/Github/cognition/vignettes/course_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB4B4FA-8E08-7A46-94AF-E16CF6022BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290D17E7-6F19-EF4E-8B74-6623B2944195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="500" windowWidth="27840" windowHeight="16620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,15 +123,6 @@
     <t>[Reading Chpt 6](https://www.crumplab.com/cognition/textbook/behaviorism.html)</t>
   </si>
   <si>
-    <t>Information Processing</t>
-  </si>
-  <si>
-    <t>Memory I</t>
-  </si>
-  <si>
-    <t>Memory II</t>
-  </si>
-  <si>
     <t>[Reading Chpt 7](https://www.crumplab.com/cognition/textbook/information-processing.html)</t>
   </si>
   <si>
@@ -141,9 +132,6 @@
     <t>[Reading Chpt 9](https://www.crumplab.com/cognition/textbook/memory-ii.html)</t>
   </si>
   <si>
-    <t xml:space="preserve">Implicit Cognition </t>
-  </si>
-  <si>
     <t>(reading on Blackboard)</t>
   </si>
   <si>
@@ -166,6 +154,18 @@
   </si>
   <si>
     <t>[Behaviorism](https://www.crumplab.com/cognition/articles/modules/L5_Behaviorism.html)</t>
+  </si>
+  <si>
+    <t>[Information Processing](https://www.crumplab.com/cognition/articles/modules/L6_Information_processing.html)</t>
+  </si>
+  <si>
+    <t>[Memory I](https://www.crumplab.com/cognition/articles/modules/L7_Memory_I.html)</t>
+  </si>
+  <si>
+    <t>[Memory II](https://www.crumplab.com/cognition/articles/modules/L8_Memory_II.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Implicit Cognition](https://www.crumplab.com/cognition/articles/modules/L9_Implicit_Cognition.html) </t>
   </si>
 </sst>
 </file>
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,7 +549,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>27</v>
@@ -563,7 +563,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>28</v>
@@ -577,7 +577,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>29</v>
@@ -591,7 +591,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>30</v>
@@ -616,10 +616,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -631,10 +631,10 @@
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="85" x14ac:dyDescent="0.2">
@@ -645,13 +645,13 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -659,10 +659,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -692,10 +692,10 @@
         <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -706,10 +706,10 @@
         <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -720,10 +720,10 @@
         <v>18</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E17" s="1"/>
     </row>

</xml_diff>